<commit_message>
1. update all addresses 2. finish A1-A6
</commit_message>
<xml_diff>
--- a/williamqiao/evidence.xlsx
+++ b/williamqiao/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Work/crypto/gon-evidence/williamqiao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Work/crypto/gon/gon-evidence/williamqiao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7C708-64D6-F545-94FE-2ADA7E0AD093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362A2C50-8B14-E146-AB5C-ADAED2FCD31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="3100" windowWidth="25680" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="2920" windowWidth="25680" windowHeight="14920" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="48">
   <si>
     <t>TeamName</t>
   </si>
@@ -132,27 +132,85 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>omniflix1t7ep36j4za4nd30ctlvc9qvf6nt5gaglvqcfrj</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>iaa1t7ep36j4za4nd30ctlvc9qvf6nt5gaglyufpka</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stars1t7ep36j4za4nd30ctlvc9qvf6nt5gagl9z7dla</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>juno1t7ep36j4za4nd30ctlvc9qvf6nt5gagl8v2tns</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>uptick1t7ep36j4za4nd30ctlvc9qvf6nt5gaglzc4tda</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>TWT#6605</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iaa103pz3cah5cqluek895wh92z9u4v9mf9qy6cjnf</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars103pz3cah5cqluek895wh92z9u4v9mf9q9y076f</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>juno103pz3cah5cqluek895wh92z9u4v9mf9q82mcky</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick1u9mvlqedr8sfk7u2ndzutlvh3vpdf8fz4tz02y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>omniflix103pz3cah5cqluek895wh92z9u4v9mf9qvxf6xx</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>32FCF0E990567BD5CDFF401C82C97A42FEBA782FE168D69464E4111165AAB0EA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>twt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C169C8C5F90CBC483BD37B6D23EFAFB84EAE1835F8D5D8393B5E14D71BA3B08A</t>
+  </si>
+  <si>
+    <t>twt0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>B0D8B0E30FE0FB1BCA827666F1E5367BF89B5E24E30878834D9F68F4CDA2C292</t>
+  </si>
+  <si>
+    <t>twt1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C0629302DEAABF9EA4F22CD7312BD5F9417CF2EE9F059FF92602FC1AE71CBA7</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars1tqrpzspyekpun2ea8wedhvm5whzshvgzjpuz3nskjlvm89z0redqwjhgq9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C4939EC38E6DAABDBBB13D2250BFCD890072ADE52A006F81E8EC4F5C12D4B7BF</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/9B6AEEB04A78AAD2EC372136EF89526996C75FAF8F5C271AEF252AD9DE74EB27</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>22EBB03786C6B2EBD50A24EBA014358AAD80BF674B02CF836DD78774DA64263E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dest chain id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>98EBF9E5C47FEE16F640014BAEFA124D5FE14585C0701D724C3086B06CBBE2A4</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -160,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -184,6 +242,12 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,12 +282,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -569,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -627,10 +692,10 @@
         <v>31</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>23</v>
@@ -1045,9 +1110,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1068,6 +1135,14 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1309,9 +1384,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1341,6 +1418,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="14">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1350,9 +1449,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1385,7 +1486,21 @@
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1397,13 +1512,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="79.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1435,6 +1553,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1444,13 +1576,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="2" max="2" width="78.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1482,6 +1617,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1491,14 +1640,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="79.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
@@ -1529,6 +1680,20 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: (evidence format error): task evidence format is incorrect
</commit_message>
<xml_diff>
--- a/williamqiao/evidence.xlsx
+++ b/williamqiao/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Work/crypto/gon/gon-evidence/williamqiao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236A21C-2E6F-4040-9ABD-C015559B1E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2344A0BB-6A74-C145-9F59-CC9C4A72D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30920" yWindow="6640" windowWidth="25680" windowHeight="14920" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16840" yWindow="9860" windowWidth="25680" windowHeight="14920" tabRatio="500" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
   <si>
     <t>TeamName</t>
   </si>
@@ -79,36 +79,12 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -209,10 +185,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>dest chain id</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>98EBF9E5C47FEE16F640014BAEFA124D5FE14585C0701D724C3086B06CBBE2A4</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -323,10 +295,6 @@
   </si>
   <si>
     <t>ibc/1543C1E1BB66932372EC8C46FCC2BF1152D1AC555C194AE1E1CA415544FD18DD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -579,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -589,7 +557,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -955,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -964,10 +931,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -978,28 +945,28 @@
     </row>
     <row r="2" spans="1:8" ht="14">
       <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1011,10 +978,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1027,23 +994,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1055,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1071,23 +1030,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1099,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1115,23 +1066,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1143,9 +1086,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
   <cols>
@@ -1157,23 +1102,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1196,42 +1133,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15">
       <c r="A3" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1259,39 +1196,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1319,39 +1256,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1379,39 +1316,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1439,39 +1376,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1499,39 +1436,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1543,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1564,18 +1501,10 @@
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1516,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -1603,59 +1532,56 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14">
       <c r="A7" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="7"/>
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1682,55 +1608,55 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1744,7 +1670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
@@ -1755,12 +1683,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1791,12 +1719,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1827,12 +1755,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1863,12 +1791,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1884,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -1904,128 +1832,128 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14">
       <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14">
       <c r="A5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14">
       <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14">
       <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14">
       <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14">
       <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14">
       <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14">
       <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14">
       <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14">
@@ -2033,76 +1961,65 @@
         <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14">
       <c r="A14" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14">
-      <c r="A16" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>91</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2114,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -2134,38 +2051,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2177,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -2198,38 +2101,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2130,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2262,38 +2151,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2305,7 +2180,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -2327,38 +2202,24 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2370,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -2386,23 +2247,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2414,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -2430,23 +2283,15 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Failed B1 (Directly transfer nft from omniflix to last owner, can not revert) Done B2
</commit_message>
<xml_diff>
--- a/williamqiao/evidence.xlsx
+++ b/williamqiao/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Work/crypto/gon/gon-evidence/williamqiao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2344A0BB-6A74-C145-9F59-CC9C4A72D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96908EC5-C385-8D4D-8541-3B80680A2214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="9860" windowWidth="25680" windowHeight="14920" tabRatio="500" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16840" yWindow="9860" windowWidth="25680" windowHeight="14920" tabRatio="500" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
   <si>
     <t>TeamName</t>
   </si>
@@ -476,6 +476,22 @@
   </si>
   <si>
     <t>TxHash</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>884C9E67BCD97226478501E25C3A51D41034703E2499E59F78F7128BF1DB39DE</t>
+  </si>
+  <si>
+    <t>5114BEE18EB4D9B147A05C74DC368BA6063F7FEDC87FA0D19155C1870FF9D155</t>
+  </si>
+  <si>
+    <t>0F629E8F140B680FEFCF4A3A055150EC13EEBD9CACD91B3084F5FFAC01B3AE97</t>
+  </si>
+  <si>
+    <t>893C21D3AB47EE67C230467A7FA6CA0DB880B36C88EDF506ABF9AF43C396ED6B</t>
+  </si>
+  <si>
+    <t>directly tranfer from omoniflix to iaa1488wwr235vka7j722hzacpk0plxw33ksqyneuz</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -902,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1668,27 +1684,33 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14">
+  <cols>
+    <col min="1" max="1" width="77" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" customHeight="1">
+    <row r="2" spans="1:2" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14">
+      <c r="A3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1706,11 +1728,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="77.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14">
       <c r="A1" s="1" t="s">
@@ -1719,12 +1744,12 @@
     </row>
     <row r="2" spans="1:1" ht="14">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
+      <c r="A3" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>